<commit_message>
old version bug fixed
</commit_message>
<xml_diff>
--- a/Cam7calib.xlsx
+++ b/Cam7calib.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127812A9-D69D-473C-A746-D2DC503D84CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C40D40D-CE54-4441-9B23-81C17E5B65D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14434" yWindow="1346" windowWidth="24686" windowHeight="13217" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1063" yWindow="1063" windowWidth="24686" windowHeight="13217" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -345,20 +345,20 @@
   <dimension ref="A1:D276"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D90"/>
+      <selection sqref="A1:D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1">
-        <v>878.97500000000002</v>
+        <v>878.39700000000005</v>
       </c>
       <c r="B1" s="1">
-        <v>1030.854</v>
+        <v>1030.5630000000001</v>
       </c>
       <c r="C1" s="1">
-        <v>2503.8000000000002</v>
+        <v>2497.3000000000002</v>
       </c>
       <c r="D1" s="1">
         <v>0</v>
@@ -366,181 +366,181 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>895.02700000000004</v>
+        <v>890.28200000000004</v>
       </c>
       <c r="B2" s="1">
-        <v>1841.8510000000001</v>
+        <v>1808.741</v>
       </c>
       <c r="C2" s="1">
-        <v>2503.8000000000002</v>
+        <v>2497.3000000000002</v>
       </c>
       <c r="D2" s="1">
-        <v>-15.92</v>
+        <v>-15.97</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>890.82600000000002</v>
+        <v>886.77700000000004</v>
       </c>
       <c r="B3" s="1">
-        <v>1741.251</v>
+        <v>1710.3710000000001</v>
       </c>
       <c r="C3" s="1">
-        <v>2503.8000000000002</v>
+        <v>2497.3000000000002</v>
       </c>
       <c r="D3" s="1">
-        <v>-14.1</v>
+        <v>-14.08</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>886.899</v>
+        <v>883.33699999999999</v>
       </c>
       <c r="B4" s="1">
-        <v>1635.6320000000001</v>
+        <v>1606.3869999999999</v>
       </c>
       <c r="C4" s="1">
-        <v>2503.8000000000002</v>
+        <v>2497.3000000000002</v>
       </c>
       <c r="D4" s="1">
-        <v>-12.1</v>
+        <v>-12.03</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>883.779</v>
+        <v>881.02200000000005</v>
       </c>
       <c r="B5" s="1">
-        <v>1532.47</v>
+        <v>1507.386</v>
       </c>
       <c r="C5" s="1">
-        <v>2503.8000000000002</v>
+        <v>2497.3000000000002</v>
       </c>
       <c r="D5" s="1">
-        <v>-10.1</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
-        <v>881.50300000000004</v>
+        <v>879.30700000000002</v>
       </c>
       <c r="B6" s="1">
-        <v>1429.729</v>
+        <v>1410.1479999999999</v>
       </c>
       <c r="C6" s="1">
-        <v>2503.8000000000002</v>
+        <v>2497.3000000000002</v>
       </c>
       <c r="D6" s="1">
-        <v>-8.1</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>879.91200000000003</v>
+        <v>878.48199999999997</v>
       </c>
       <c r="B7" s="1">
-        <v>1328.54</v>
+        <v>1313.383</v>
       </c>
       <c r="C7" s="1">
-        <v>2503.8000000000002</v>
+        <v>2497.3000000000002</v>
       </c>
       <c r="D7" s="1">
-        <v>-6.07</v>
+        <v>-5.97</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
-        <v>878.97799999999995</v>
+        <v>877.61300000000006</v>
       </c>
       <c r="B8" s="1">
-        <v>1228.7850000000001</v>
+        <v>1218.48</v>
       </c>
       <c r="C8" s="1">
-        <v>2503.8000000000002</v>
+        <v>2497.3000000000002</v>
       </c>
       <c r="D8" s="1">
-        <v>-4.05</v>
+        <v>-3.97</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <v>878.529</v>
+        <v>877.78300000000002</v>
       </c>
       <c r="B9" s="1">
-        <v>1130.5730000000001</v>
+        <v>1124.7919999999999</v>
       </c>
       <c r="C9" s="1">
-        <v>2503.8000000000002</v>
+        <v>2497.3000000000002</v>
       </c>
       <c r="D9" s="1">
-        <v>-2.02</v>
+        <v>-1.97</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
-        <v>878.875</v>
+        <v>878.41</v>
       </c>
       <c r="B10" s="1">
-        <v>1034.7139999999999</v>
+        <v>1030.69</v>
       </c>
       <c r="C10" s="1">
-        <v>2503.8000000000002</v>
+        <v>2497.3000000000002</v>
       </c>
       <c r="D10" s="1">
-        <v>-0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <v>880.048</v>
+        <v>879.83199999999999</v>
       </c>
       <c r="B11" s="1">
-        <v>937.17700000000002</v>
+        <v>935.75099999999998</v>
       </c>
       <c r="C11" s="1">
-        <v>2503.8000000000002</v>
+        <v>2497.3000000000002</v>
       </c>
       <c r="D11" s="1">
-        <v>1.98</v>
+        <v>2.0299999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
-        <v>881.58500000000004</v>
+        <v>881.52300000000002</v>
       </c>
       <c r="B12" s="1">
-        <v>840.70799999999997</v>
+        <v>841.06299999999999</v>
       </c>
       <c r="C12" s="1">
-        <v>2503.8000000000002</v>
+        <v>2497.3000000000002</v>
       </c>
       <c r="D12" s="1">
-        <v>3.98</v>
+        <v>4.03</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>884.11500000000001</v>
+        <v>884</v>
       </c>
       <c r="B13" s="1">
-        <v>744.14700000000005</v>
+        <v>746.99800000000005</v>
       </c>
       <c r="C13" s="1">
-        <v>2503.8000000000002</v>
+        <v>2497.3000000000002</v>
       </c>
       <c r="D13" s="1">
-        <v>5.98</v>
+        <v>6.03</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
-        <v>887.08500000000004</v>
+        <v>887.00800000000004</v>
       </c>
       <c r="B14" s="1">
-        <v>646.94000000000005</v>
+        <v>652.05899999999997</v>
       </c>
       <c r="C14" s="1">
-        <v>2503.8000000000002</v>
+        <v>2497.3000000000002</v>
       </c>
       <c r="D14" s="1">
         <v>8.0299999999999994</v>
@@ -548,13 +548,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
-        <v>890.61099999999999</v>
+        <v>890.54100000000005</v>
       </c>
       <c r="B15" s="1">
-        <v>550.59400000000005</v>
+        <v>556.12400000000002</v>
       </c>
       <c r="C15" s="1">
-        <v>2503.8000000000002</v>
+        <v>2497.3000000000002</v>
       </c>
       <c r="D15" s="1">
         <v>10.029999999999999</v>
@@ -562,27 +562,27 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
-        <v>894.93</v>
+        <v>894.654</v>
       </c>
       <c r="B16" s="1">
-        <v>453.49799999999999</v>
+        <v>459.10899999999998</v>
       </c>
       <c r="C16" s="1">
-        <v>2503.8000000000002</v>
+        <v>2497.3000000000002</v>
       </c>
       <c r="D16" s="1">
-        <v>12</v>
+        <v>12.03</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
-        <v>899.99199999999996</v>
+        <v>899.48800000000006</v>
       </c>
       <c r="B17" s="1">
-        <v>353.517</v>
+        <v>360.32799999999997</v>
       </c>
       <c r="C17" s="1">
-        <v>2503.8000000000002</v>
+        <v>2497.3000000000002</v>
       </c>
       <c r="D17" s="1">
         <v>14.03</v>
@@ -590,13 +590,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
-        <v>905.50599999999997</v>
+        <v>904.66</v>
       </c>
       <c r="B18" s="1">
-        <v>253.631</v>
+        <v>261.10000000000002</v>
       </c>
       <c r="C18" s="1">
-        <v>2503.8000000000002</v>
+        <v>2497.3000000000002</v>
       </c>
       <c r="D18" s="1">
         <v>16.03</v>
@@ -604,13 +604,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
-        <v>860.08699999999999</v>
+        <v>859.52800000000002</v>
       </c>
       <c r="B19" s="1">
-        <v>1030.7349999999999</v>
+        <v>1030.6690000000001</v>
       </c>
       <c r="C19" s="1">
-        <v>2603.5</v>
+        <v>2597</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
@@ -618,181 +618,181 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
-        <v>875.298</v>
+        <v>870.53800000000001</v>
       </c>
       <c r="B20" s="1">
-        <v>1839.4349999999999</v>
+        <v>1809.029</v>
       </c>
       <c r="C20" s="1">
-        <v>2603.5</v>
+        <v>2597</v>
       </c>
       <c r="D20" s="1">
-        <v>-15.92</v>
+        <v>-15.97</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
-        <v>871.19299999999998</v>
+        <v>867.18100000000004</v>
       </c>
       <c r="B21" s="1">
-        <v>1738.9190000000001</v>
+        <v>1710.1469999999999</v>
       </c>
       <c r="C21" s="1">
-        <v>2603.5</v>
+        <v>2597</v>
       </c>
       <c r="D21" s="1">
-        <v>-14.1</v>
+        <v>-14.05</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
-        <v>867.53</v>
+        <v>864.11599999999999</v>
       </c>
       <c r="B22" s="1">
-        <v>1633.588</v>
+        <v>1607.6279999999999</v>
       </c>
       <c r="C22" s="1">
-        <v>2603.5</v>
+        <v>2597</v>
       </c>
       <c r="D22" s="1">
-        <v>-12.1</v>
+        <v>-12.03</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
-        <v>864.65700000000004</v>
+        <v>861.91300000000001</v>
       </c>
       <c r="B23" s="1">
-        <v>1529.665</v>
+        <v>1508.749</v>
       </c>
       <c r="C23" s="1">
-        <v>2603.5</v>
+        <v>2597</v>
       </c>
       <c r="D23" s="1">
-        <v>-10.1</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
-        <v>862.34400000000005</v>
+        <v>860.22</v>
       </c>
       <c r="B24" s="1">
-        <v>1427.355</v>
+        <v>1410.4760000000001</v>
       </c>
       <c r="C24" s="1">
-        <v>2603.5</v>
+        <v>2597</v>
       </c>
       <c r="D24" s="1">
-        <v>-8.1</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
-        <v>860.952</v>
+        <v>859.46299999999997</v>
       </c>
       <c r="B25" s="1">
-        <v>1326.569</v>
+        <v>1315.2660000000001</v>
       </c>
       <c r="C25" s="1">
-        <v>2603.5</v>
+        <v>2597</v>
       </c>
       <c r="D25" s="1">
-        <v>-6.05</v>
+        <v>-5.97</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
-        <v>860.06200000000001</v>
+        <v>858.64</v>
       </c>
       <c r="B26" s="1">
-        <v>1227.67</v>
+        <v>1219.857</v>
       </c>
       <c r="C26" s="1">
-        <v>2603.5</v>
+        <v>2597</v>
       </c>
       <c r="D26" s="1">
-        <v>-4.07</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
-        <v>859.63099999999997</v>
+        <v>858.90200000000004</v>
       </c>
       <c r="B27" s="1">
-        <v>1128.7380000000001</v>
+        <v>1124.5930000000001</v>
       </c>
       <c r="C27" s="1">
-        <v>2603.5</v>
+        <v>2597</v>
       </c>
       <c r="D27" s="1">
-        <v>-2.02</v>
+        <v>-1.97</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
-        <v>860.09799999999996</v>
+        <v>859.46600000000001</v>
       </c>
       <c r="B28" s="1">
-        <v>1033.4490000000001</v>
+        <v>1030.711</v>
       </c>
       <c r="C28" s="1">
-        <v>2603.5</v>
+        <v>2597</v>
       </c>
       <c r="D28" s="1">
-        <v>-0.05</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
-        <v>861.14599999999996</v>
+        <v>860.82399999999996</v>
       </c>
       <c r="B29" s="1">
-        <v>935.84400000000005</v>
+        <v>937.27</v>
       </c>
       <c r="C29" s="1">
-        <v>2603.5</v>
+        <v>2597</v>
       </c>
       <c r="D29" s="1">
-        <v>1.98</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
-        <v>862.70100000000002</v>
+        <v>862.48400000000004</v>
       </c>
       <c r="B30" s="1">
-        <v>839.44799999999998</v>
+        <v>841.74199999999996</v>
       </c>
       <c r="C30" s="1">
-        <v>2603.5</v>
+        <v>2597</v>
       </c>
       <c r="D30" s="1">
-        <v>3.98</v>
+        <v>4.05</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
-        <v>865.11900000000003</v>
+        <v>864.96500000000003</v>
       </c>
       <c r="B31" s="1">
-        <v>742.54100000000005</v>
+        <v>748.74300000000005</v>
       </c>
       <c r="C31" s="1">
-        <v>2603.5</v>
+        <v>2597</v>
       </c>
       <c r="D31" s="1">
-        <v>5.98</v>
+        <v>6.03</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
-        <v>868.072</v>
+        <v>867.92899999999997</v>
       </c>
       <c r="B32" s="1">
-        <v>645.70899999999995</v>
+        <v>653.83699999999999</v>
       </c>
       <c r="C32" s="1">
-        <v>2603.5</v>
+        <v>2597</v>
       </c>
       <c r="D32" s="1">
         <v>8.0299999999999994</v>
@@ -800,13 +800,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
-        <v>871.53700000000003</v>
+        <v>871.29499999999996</v>
       </c>
       <c r="B33" s="1">
-        <v>549.649</v>
+        <v>558.52300000000002</v>
       </c>
       <c r="C33" s="1">
-        <v>2603.5</v>
+        <v>2597</v>
       </c>
       <c r="D33" s="1">
         <v>10.029999999999999</v>
@@ -814,41 +814,41 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
-        <v>875.62199999999996</v>
+        <v>875.47</v>
       </c>
       <c r="B34" s="1">
-        <v>452.88</v>
+        <v>460.92</v>
       </c>
       <c r="C34" s="1">
-        <v>2603.5</v>
+        <v>2597</v>
       </c>
       <c r="D34" s="1">
-        <v>12</v>
+        <v>12.03</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
-        <v>880.67700000000002</v>
+        <v>879.745</v>
       </c>
       <c r="B35" s="1">
-        <v>352.98399999999998</v>
+        <v>363.19200000000001</v>
       </c>
       <c r="C35" s="1">
-        <v>2603.5</v>
+        <v>2597</v>
       </c>
       <c r="D35" s="1">
-        <v>14.05</v>
+        <v>14.03</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
-        <v>886.05200000000002</v>
+        <v>885.05200000000002</v>
       </c>
       <c r="B36" s="1">
-        <v>254.29599999999999</v>
+        <v>263.13400000000001</v>
       </c>
       <c r="C36" s="1">
-        <v>2603.5</v>
+        <v>2597</v>
       </c>
       <c r="D36" s="1">
         <v>16</v>
@@ -856,13 +856,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
-        <v>842.803</v>
+        <v>841.99400000000003</v>
       </c>
       <c r="B37" s="1">
-        <v>1030.663</v>
+        <v>1030.4580000000001</v>
       </c>
       <c r="C37" s="1">
-        <v>2703.2</v>
+        <v>2696.7</v>
       </c>
       <c r="D37" s="1">
         <v>0</v>
@@ -870,251 +870,251 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
-        <v>857.00099999999998</v>
+        <v>852.46100000000001</v>
       </c>
       <c r="B38" s="1">
-        <v>1837.3630000000001</v>
+        <v>1807.742</v>
       </c>
       <c r="C38" s="1">
-        <v>2703.2</v>
+        <v>2696.7</v>
       </c>
       <c r="D38" s="1">
-        <v>-15.92</v>
+        <v>-15.98</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
-        <v>853.21600000000001</v>
+        <v>849.18299999999999</v>
       </c>
       <c r="B39" s="1">
-        <v>1737.4380000000001</v>
+        <v>1708.502</v>
       </c>
       <c r="C39" s="1">
-        <v>2703.2</v>
+        <v>2696.7</v>
       </c>
       <c r="D39" s="1">
-        <v>-14.1</v>
+        <v>-14.05</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
-        <v>849.80200000000002</v>
+        <v>846.25099999999998</v>
       </c>
       <c r="B40" s="1">
-        <v>1633.05</v>
+        <v>1606.3489999999999</v>
       </c>
       <c r="C40" s="1">
-        <v>2703.2</v>
+        <v>2696.7</v>
       </c>
       <c r="D40" s="1">
-        <v>-12.1</v>
+        <v>-12.03</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
-        <v>846.98400000000004</v>
+        <v>844.06</v>
       </c>
       <c r="B41" s="1">
-        <v>1528.0609999999999</v>
+        <v>1506.846</v>
       </c>
       <c r="C41" s="1">
-        <v>2703.2</v>
+        <v>2696.7</v>
       </c>
       <c r="D41" s="1">
-        <v>-10.1</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
-        <v>844.93399999999997</v>
+        <v>842.51900000000001</v>
       </c>
       <c r="B42" s="1">
-        <v>1426.4059999999999</v>
+        <v>1410.377</v>
       </c>
       <c r="C42" s="1">
-        <v>2703.2</v>
+        <v>2696.7</v>
       </c>
       <c r="D42" s="1">
-        <v>-8.1</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
-        <v>843.21299999999997</v>
+        <v>841.56700000000001</v>
       </c>
       <c r="B43" s="1">
-        <v>1325.3040000000001</v>
+        <v>1314.184</v>
       </c>
       <c r="C43" s="1">
-        <v>2703.2</v>
+        <v>2696.7</v>
       </c>
       <c r="D43" s="1">
-        <v>-6.05</v>
+        <v>-5.98</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
-        <v>842.54899999999998</v>
+        <v>841.28499999999997</v>
       </c>
       <c r="B44" s="1">
-        <v>1226.6379999999999</v>
+        <v>1218.932</v>
       </c>
       <c r="C44" s="1">
-        <v>2703.2</v>
+        <v>2696.7</v>
       </c>
       <c r="D44" s="1">
-        <v>-4.07</v>
+        <v>-3.98</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
-        <v>842.46400000000006</v>
+        <v>841.23599999999999</v>
       </c>
       <c r="B45" s="1">
-        <v>1128.2049999999999</v>
+        <v>1124.75</v>
       </c>
       <c r="C45" s="1">
-        <v>2703.2</v>
+        <v>2696.7</v>
       </c>
       <c r="D45" s="1">
-        <v>-2.02</v>
+        <v>-1.98</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
-        <v>842.79300000000001</v>
+        <v>841.99400000000003</v>
       </c>
       <c r="B46" s="1">
-        <v>1032.8409999999999</v>
+        <v>1031.4010000000001</v>
       </c>
       <c r="C46" s="1">
-        <v>2703.2</v>
+        <v>2696.7</v>
       </c>
       <c r="D46" s="1">
-        <v>-0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
-        <v>843.85</v>
+        <v>843.077</v>
       </c>
       <c r="B47" s="1">
-        <v>935.16499999999996</v>
+        <v>936.51300000000003</v>
       </c>
       <c r="C47" s="1">
-        <v>2703.2</v>
+        <v>2696.7</v>
       </c>
       <c r="D47" s="1">
-        <v>1.98</v>
+        <v>2.02</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
-        <v>845.47299999999996</v>
+        <v>845.00099999999998</v>
       </c>
       <c r="B48" s="1">
-        <v>838.63300000000004</v>
+        <v>842.44299999999998</v>
       </c>
       <c r="C48" s="1">
-        <v>2703.2</v>
+        <v>2696.7</v>
       </c>
       <c r="D48" s="1">
-        <v>3.98</v>
+        <v>4.0199999999999996</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
-        <v>847.74599999999998</v>
+        <v>847.09100000000001</v>
       </c>
       <c r="B49" s="1">
-        <v>742.27700000000004</v>
+        <v>748.77599999999995</v>
       </c>
       <c r="C49" s="1">
-        <v>2703.2</v>
+        <v>2696.7</v>
       </c>
       <c r="D49" s="1">
-        <v>6</v>
+        <v>6.02</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
-        <v>850.55700000000002</v>
+        <v>850.09100000000001</v>
       </c>
       <c r="B50" s="1">
-        <v>645.76199999999994</v>
+        <v>653.44799999999998</v>
       </c>
       <c r="C50" s="1">
-        <v>2703.2</v>
+        <v>2696.7</v>
       </c>
       <c r="D50" s="1">
-        <v>8</v>
+        <v>8.02</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
-        <v>854.07</v>
+        <v>853.5</v>
       </c>
       <c r="B51" s="1">
-        <v>549.26499999999999</v>
+        <v>557.26099999999997</v>
       </c>
       <c r="C51" s="1">
-        <v>2703.2</v>
+        <v>2696.7</v>
       </c>
       <c r="D51" s="1">
-        <v>10.029999999999999</v>
+        <v>10.050000000000001</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
-        <v>857.93499999999995</v>
+        <v>857.47199999999998</v>
       </c>
       <c r="B52" s="1">
-        <v>452.803</v>
+        <v>461.74</v>
       </c>
       <c r="C52" s="1">
-        <v>2703.2</v>
+        <v>2696.7</v>
       </c>
       <c r="D52" s="1">
-        <v>12.03</v>
+        <v>12.02</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
-        <v>862.75300000000004</v>
+        <v>861.71699999999998</v>
       </c>
       <c r="B53" s="1">
-        <v>354.37400000000002</v>
+        <v>364.017</v>
       </c>
       <c r="C53" s="1">
-        <v>2703.2</v>
+        <v>2696.7</v>
       </c>
       <c r="D53" s="1">
-        <v>14.03</v>
+        <v>14.02</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
-        <v>867.87800000000004</v>
+        <v>866.73199999999997</v>
       </c>
       <c r="B54" s="1">
-        <v>254.91</v>
+        <v>263.37299999999999</v>
       </c>
       <c r="C54" s="1">
-        <v>2703.2</v>
+        <v>2696.7</v>
       </c>
       <c r="D54" s="1">
-        <v>16</v>
+        <v>16.02</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
-        <v>826.64</v>
+        <v>825.90499999999997</v>
       </c>
       <c r="B55" s="1">
-        <v>1030.8969999999999</v>
+        <v>1030.9359999999999</v>
       </c>
       <c r="C55" s="1">
-        <v>2802.9</v>
+        <v>2796.4</v>
       </c>
       <c r="D55" s="1">
         <v>0</v>
@@ -1122,251 +1122,251 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
-        <v>840.096</v>
+        <v>835.56399999999996</v>
       </c>
       <c r="B56" s="1">
-        <v>1835.1559999999999</v>
+        <v>1806.346</v>
       </c>
       <c r="C56" s="1">
-        <v>2802.9</v>
+        <v>2796.4</v>
       </c>
       <c r="D56" s="1">
-        <v>-15.9</v>
+        <v>-15.97</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
-        <v>836.60699999999997</v>
+        <v>832.49300000000005</v>
       </c>
       <c r="B57" s="1">
-        <v>1735.992</v>
+        <v>1707.943</v>
       </c>
       <c r="C57" s="1">
-        <v>2802.9</v>
+        <v>2796.4</v>
       </c>
       <c r="D57" s="1">
-        <v>-14.08</v>
+        <v>-14.07</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
-        <v>833.18799999999999</v>
+        <v>829.51900000000001</v>
       </c>
       <c r="B58" s="1">
-        <v>1630.8389999999999</v>
+        <v>1605.0029999999999</v>
       </c>
       <c r="C58" s="1">
-        <v>2802.9</v>
+        <v>2796.4</v>
       </c>
       <c r="D58" s="1">
-        <v>-12.08</v>
+        <v>-12</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
-        <v>830.57100000000003</v>
+        <v>827.53599999999994</v>
       </c>
       <c r="B59" s="1">
-        <v>1527.5509999999999</v>
+        <v>1506.6289999999999</v>
       </c>
       <c r="C59" s="1">
-        <v>2802.9</v>
+        <v>2796.4</v>
       </c>
       <c r="D59" s="1">
-        <v>-10.08</v>
+        <v>-10.02</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
-        <v>828.6</v>
+        <v>826.25800000000004</v>
       </c>
       <c r="B60" s="1">
-        <v>1426.451</v>
+        <v>1409.367</v>
       </c>
       <c r="C60" s="1">
-        <v>2802.9</v>
+        <v>2796.4</v>
       </c>
       <c r="D60" s="1">
-        <v>-8.08</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
-        <v>827.08500000000004</v>
+        <v>825.41099999999994</v>
       </c>
       <c r="B61" s="1">
-        <v>1326.105</v>
+        <v>1312.665</v>
       </c>
       <c r="C61" s="1">
-        <v>2802.9</v>
+        <v>2796.4</v>
       </c>
       <c r="D61" s="1">
-        <v>-6.08</v>
+        <v>-5.97</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
-        <v>826.428</v>
+        <v>824.96100000000001</v>
       </c>
       <c r="B62" s="1">
-        <v>1226.6210000000001</v>
+        <v>1219.018</v>
       </c>
       <c r="C62" s="1">
-        <v>2802.9</v>
+        <v>2796.4</v>
       </c>
       <c r="D62" s="1">
-        <v>-4.05</v>
+        <v>-3.97</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
-        <v>826.12</v>
+        <v>825</v>
       </c>
       <c r="B63" s="1">
-        <v>1129.758</v>
+        <v>1124.7829999999999</v>
       </c>
       <c r="C63" s="1">
-        <v>2802.9</v>
+        <v>2796.4</v>
       </c>
       <c r="D63" s="1">
-        <v>-2.0499999999999998</v>
+        <v>-1.97</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
-        <v>826.68700000000001</v>
+        <v>825.90300000000002</v>
       </c>
       <c r="B64" s="1">
-        <v>1032.2629999999999</v>
+        <v>1031.077</v>
       </c>
       <c r="C64" s="1">
-        <v>2802.9</v>
+        <v>2796.4</v>
       </c>
       <c r="D64" s="1">
-        <v>-0.03</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
-        <v>827.577</v>
+        <v>826.98800000000006</v>
       </c>
       <c r="B65" s="1">
-        <v>936.11599999999999</v>
+        <v>936.71600000000001</v>
       </c>
       <c r="C65" s="1">
-        <v>2802.9</v>
+        <v>2796.4</v>
       </c>
       <c r="D65" s="1">
-        <v>1.95</v>
+        <v>2.0299999999999998</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
-        <v>829.32100000000003</v>
+        <v>828.83100000000002</v>
       </c>
       <c r="B66" s="1">
-        <v>838.69399999999996</v>
+        <v>842.41700000000003</v>
       </c>
       <c r="C66" s="1">
-        <v>2802.9</v>
+        <v>2796.4</v>
       </c>
       <c r="D66" s="1">
-        <v>4</v>
+        <v>4.03</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
-        <v>831.49300000000005</v>
+        <v>831.02300000000002</v>
       </c>
       <c r="B67" s="1">
-        <v>743.197</v>
+        <v>748.01300000000003</v>
       </c>
       <c r="C67" s="1">
-        <v>2802.9</v>
+        <v>2796.4</v>
       </c>
       <c r="D67" s="1">
-        <v>6</v>
+        <v>6.03</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
-        <v>834.23900000000003</v>
+        <v>833.88199999999995</v>
       </c>
       <c r="B68" s="1">
-        <v>646.88300000000004</v>
+        <v>653.44100000000003</v>
       </c>
       <c r="C68" s="1">
-        <v>2802.9</v>
+        <v>2796.4</v>
       </c>
       <c r="D68" s="1">
-        <v>8</v>
+        <v>8.0299999999999994</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
-        <v>837.55799999999999</v>
+        <v>837.10400000000004</v>
       </c>
       <c r="B69" s="1">
-        <v>550.19899999999996</v>
+        <v>558.072</v>
       </c>
       <c r="C69" s="1">
-        <v>2802.9</v>
+        <v>2796.4</v>
       </c>
       <c r="D69" s="1">
-        <v>10.02</v>
+        <v>10.029999999999999</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
-        <v>841.70899999999995</v>
+        <v>840.678</v>
       </c>
       <c r="B70" s="1">
-        <v>453.49400000000003</v>
+        <v>461.69200000000001</v>
       </c>
       <c r="C70" s="1">
-        <v>2802.9</v>
+        <v>2796.4</v>
       </c>
       <c r="D70" s="1">
-        <v>12.02</v>
+        <v>12.03</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
-        <v>846.02300000000002</v>
+        <v>845.29</v>
       </c>
       <c r="B71" s="1">
-        <v>355.80700000000002</v>
+        <v>363.05900000000003</v>
       </c>
       <c r="C71" s="1">
-        <v>2802.9</v>
+        <v>2796.4</v>
       </c>
       <c r="D71" s="1">
-        <v>14.02</v>
+        <v>14.03</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
-        <v>851.25099999999998</v>
+        <v>849.87300000000005</v>
       </c>
       <c r="B72" s="1">
-        <v>255.40100000000001</v>
+        <v>263.92899999999997</v>
       </c>
       <c r="C72" s="1">
-        <v>2802.9</v>
+        <v>2796.4</v>
       </c>
       <c r="D72" s="1">
-        <v>16.02</v>
+        <v>16.03</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
-        <v>811.72500000000002</v>
+        <v>810.80499999999995</v>
       </c>
       <c r="B73" s="1">
-        <v>1030.7570000000001</v>
+        <v>1030.646</v>
       </c>
       <c r="C73" s="1">
-        <v>2902.6</v>
+        <v>2896.1</v>
       </c>
       <c r="D73" s="1">
         <v>0</v>
@@ -1374,167 +1374,167 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
-        <v>824.625</v>
+        <v>819.94500000000005</v>
       </c>
       <c r="B74" s="1">
-        <v>1834.66</v>
+        <v>1805.9960000000001</v>
       </c>
       <c r="C74" s="1">
-        <v>2902.6</v>
+        <v>2896.1</v>
       </c>
       <c r="D74" s="1">
-        <v>-15.9</v>
+        <v>-16</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
-        <v>821.11199999999997</v>
+        <v>816.91899999999998</v>
       </c>
       <c r="B75" s="1">
-        <v>1735.3979999999999</v>
+        <v>1705.932</v>
       </c>
       <c r="C75" s="1">
-        <v>2902.6</v>
+        <v>2896.1</v>
       </c>
       <c r="D75" s="1">
-        <v>-14.08</v>
+        <v>-14.05</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
-        <v>817.60699999999997</v>
+        <v>814.27700000000004</v>
       </c>
       <c r="B76" s="1">
-        <v>1629.318</v>
+        <v>1604.518</v>
       </c>
       <c r="C76" s="1">
-        <v>2902.6</v>
+        <v>2896.1</v>
       </c>
       <c r="D76" s="1">
-        <v>-12.08</v>
+        <v>-12.03</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
-        <v>815.35900000000004</v>
+        <v>812.35799999999995</v>
       </c>
       <c r="B77" s="1">
-        <v>1526.9359999999999</v>
+        <v>1505.5740000000001</v>
       </c>
       <c r="C77" s="1">
-        <v>2902.6</v>
+        <v>2896.1</v>
       </c>
       <c r="D77" s="1">
-        <v>-10.08</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
-        <v>813.38800000000003</v>
+        <v>811.02599999999995</v>
       </c>
       <c r="B78" s="1">
-        <v>1425.5319999999999</v>
+        <v>1409.02</v>
       </c>
       <c r="C78" s="1">
-        <v>2902.6</v>
+        <v>2896.1</v>
       </c>
       <c r="D78" s="1">
-        <v>-8.08</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
-        <v>812.17399999999998</v>
+        <v>810.37099999999998</v>
       </c>
       <c r="B79" s="1">
-        <v>1325.779</v>
+        <v>1312.8630000000001</v>
       </c>
       <c r="C79" s="1">
-        <v>2902.6</v>
+        <v>2896.1</v>
       </c>
       <c r="D79" s="1">
-        <v>-6.08</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
-        <v>811.48</v>
+        <v>809.95600000000002</v>
       </c>
       <c r="B80" s="1">
-        <v>1226.173</v>
+        <v>1217.3420000000001</v>
       </c>
       <c r="C80" s="1">
-        <v>2902.6</v>
+        <v>2896.1</v>
       </c>
       <c r="D80" s="1">
-        <v>-4.05</v>
+        <v>-3.97</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
-        <v>811.11900000000003</v>
+        <v>810.00699999999995</v>
       </c>
       <c r="B81" s="1">
-        <v>1128.521</v>
+        <v>1123.625</v>
       </c>
       <c r="C81" s="1">
-        <v>2902.6</v>
+        <v>2896.1</v>
       </c>
       <c r="D81" s="1">
-        <v>-2.0499999999999998</v>
+        <v>-1.95</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
-        <v>811.71500000000003</v>
+        <v>810.779</v>
       </c>
       <c r="B82" s="1">
-        <v>1031.934</v>
+        <v>1030.752</v>
       </c>
       <c r="C82" s="1">
-        <v>2902.6</v>
+        <v>2896.1</v>
       </c>
       <c r="D82" s="1">
-        <v>-0.03</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
-        <v>812.59900000000005</v>
+        <v>811.94899999999996</v>
       </c>
       <c r="B83" s="1">
-        <v>936.17700000000002</v>
+        <v>936.39400000000001</v>
       </c>
       <c r="C83" s="1">
-        <v>2902.6</v>
+        <v>2896.1</v>
       </c>
       <c r="D83" s="1">
-        <v>1.97</v>
+        <v>2.0299999999999998</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
-        <v>814.34900000000005</v>
+        <v>813.71299999999997</v>
       </c>
       <c r="B84" s="1">
-        <v>839.49699999999996</v>
+        <v>842.82</v>
       </c>
       <c r="C84" s="1">
-        <v>2902.6</v>
+        <v>2896.1</v>
       </c>
       <c r="D84" s="1">
-        <v>3.97</v>
+        <v>4.03</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
-        <v>816.45899999999995</v>
+        <v>815.88499999999999</v>
       </c>
       <c r="B85" s="1">
-        <v>743.36800000000005</v>
+        <v>749.39200000000005</v>
       </c>
       <c r="C85" s="1">
-        <v>2902.6</v>
+        <v>2896.1</v>
       </c>
       <c r="D85" s="1">
         <v>6</v>
@@ -1542,181 +1542,325 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
-        <v>819.20899999999995</v>
+        <v>818.58199999999999</v>
       </c>
       <c r="B86" s="1">
-        <v>647.36</v>
+        <v>652.79</v>
       </c>
       <c r="C86" s="1">
-        <v>2902.6</v>
+        <v>2896.1</v>
       </c>
       <c r="D86" s="1">
-        <v>8</v>
+        <v>8.0500000000000007</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
-        <v>822.50900000000001</v>
+        <v>821.64200000000005</v>
       </c>
       <c r="B87" s="1">
-        <v>550.24400000000003</v>
+        <v>559.03200000000004</v>
       </c>
       <c r="C87" s="1">
-        <v>2902.6</v>
+        <v>2896.1</v>
       </c>
       <c r="D87" s="1">
-        <v>10.02</v>
+        <v>10.029999999999999</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
-        <v>826.19200000000001</v>
+        <v>825.48699999999997</v>
       </c>
       <c r="B88" s="1">
-        <v>453.452</v>
+        <v>462.19499999999999</v>
       </c>
       <c r="C88" s="1">
-        <v>2902.6</v>
+        <v>2896.1</v>
       </c>
       <c r="D88" s="1">
-        <v>12.02</v>
+        <v>12.03</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
-        <v>830.71600000000001</v>
+        <v>829.529</v>
       </c>
       <c r="B89" s="1">
-        <v>355.22699999999998</v>
+        <v>364.685</v>
       </c>
       <c r="C89" s="1">
-        <v>2902.6</v>
+        <v>2896.1</v>
       </c>
       <c r="D89" s="1">
-        <v>14.02</v>
+        <v>14.03</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
-        <v>835.58</v>
+        <v>834.4</v>
       </c>
       <c r="B90" s="1">
-        <v>256.42399999999998</v>
+        <v>264.88200000000001</v>
       </c>
       <c r="C90" s="1">
-        <v>2902.6</v>
+        <v>2896.1</v>
       </c>
       <c r="D90" s="1">
-        <v>16.02</v>
+        <v>16.03</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A91" s="1"/>
-      <c r="B91" s="1"/>
-      <c r="C91" s="1"/>
-      <c r="D91" s="1"/>
+      <c r="A91" s="1">
+        <v>796.66899999999998</v>
+      </c>
+      <c r="B91" s="1">
+        <v>1030.5640000000001</v>
+      </c>
+      <c r="C91" s="1">
+        <v>2995.8</v>
+      </c>
+      <c r="D91" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A92" s="1"/>
-      <c r="B92" s="1"/>
-      <c r="C92" s="1"/>
-      <c r="D92" s="1"/>
+      <c r="A92" s="1">
+        <v>805.32399999999996</v>
+      </c>
+      <c r="B92" s="1">
+        <v>1805.0450000000001</v>
+      </c>
+      <c r="C92" s="1">
+        <v>2995.8</v>
+      </c>
+      <c r="D92" s="1">
+        <v>-15.97</v>
+      </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A93" s="1"/>
-      <c r="B93" s="1"/>
-      <c r="C93" s="1"/>
-      <c r="D93" s="1"/>
+      <c r="A93" s="1">
+        <v>802.51599999999996</v>
+      </c>
+      <c r="B93" s="1">
+        <v>1705.9079999999999</v>
+      </c>
+      <c r="C93" s="1">
+        <v>2995.8</v>
+      </c>
+      <c r="D93" s="1">
+        <v>-14.07</v>
+      </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A94" s="1"/>
-      <c r="B94" s="1"/>
-      <c r="C94" s="1"/>
-      <c r="D94" s="1"/>
+      <c r="A94" s="1">
+        <v>799.93299999999999</v>
+      </c>
+      <c r="B94" s="1">
+        <v>1603.59</v>
+      </c>
+      <c r="C94" s="1">
+        <v>2995.8</v>
+      </c>
+      <c r="D94" s="1">
+        <v>-12.03</v>
+      </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A95" s="1"/>
-      <c r="B95" s="1"/>
-      <c r="C95" s="1"/>
-      <c r="D95" s="1"/>
+      <c r="A95" s="1">
+        <v>798.15800000000002</v>
+      </c>
+      <c r="B95" s="1">
+        <v>1504.153</v>
+      </c>
+      <c r="C95" s="1">
+        <v>2995.8</v>
+      </c>
+      <c r="D95" s="1">
+        <v>-10</v>
+      </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A96" s="1"/>
-      <c r="B96" s="1"/>
-      <c r="C96" s="1"/>
-      <c r="D96" s="1"/>
+      <c r="A96" s="1">
+        <v>796.63800000000003</v>
+      </c>
+      <c r="B96" s="1">
+        <v>1407.528</v>
+      </c>
+      <c r="C96" s="1">
+        <v>2995.8</v>
+      </c>
+      <c r="D96" s="1">
+        <v>-8</v>
+      </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A97" s="1"/>
-      <c r="B97" s="1"/>
-      <c r="C97" s="1"/>
-      <c r="D97" s="1"/>
+      <c r="A97" s="1">
+        <v>796.11500000000001</v>
+      </c>
+      <c r="B97" s="1">
+        <v>1312.3820000000001</v>
+      </c>
+      <c r="C97" s="1">
+        <v>2995.8</v>
+      </c>
+      <c r="D97" s="1">
+        <v>-5.97</v>
+      </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A98" s="1"/>
-      <c r="B98" s="1"/>
-      <c r="C98" s="1"/>
-      <c r="D98" s="1"/>
+      <c r="A98" s="1">
+        <v>795.84100000000001</v>
+      </c>
+      <c r="B98" s="1">
+        <v>1217.4780000000001</v>
+      </c>
+      <c r="C98" s="1">
+        <v>2995.8</v>
+      </c>
+      <c r="D98" s="1">
+        <v>-3.97</v>
+      </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
-      <c r="C99" s="1"/>
-      <c r="D99" s="1"/>
+      <c r="A99" s="1">
+        <v>795.995</v>
+      </c>
+      <c r="B99" s="1">
+        <v>1123.7190000000001</v>
+      </c>
+      <c r="C99" s="1">
+        <v>2995.8</v>
+      </c>
+      <c r="D99" s="1">
+        <v>-1.97</v>
+      </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A100" s="1"/>
-      <c r="B100" s="1"/>
-      <c r="C100" s="1"/>
-      <c r="D100" s="1"/>
+      <c r="A100" s="1">
+        <v>796.70399999999995</v>
+      </c>
+      <c r="B100" s="1">
+        <v>1030.3779999999999</v>
+      </c>
+      <c r="C100" s="1">
+        <v>2995.8</v>
+      </c>
+      <c r="D100" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A101" s="1"/>
-      <c r="B101" s="1"/>
-      <c r="C101" s="1"/>
-      <c r="D101" s="1"/>
+      <c r="A101" s="1">
+        <v>797.923</v>
+      </c>
+      <c r="B101" s="1">
+        <v>936.06200000000001</v>
+      </c>
+      <c r="C101" s="1">
+        <v>2995.8</v>
+      </c>
+      <c r="D101" s="1">
+        <v>2.0299999999999998</v>
+      </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A102" s="1"/>
-      <c r="B102" s="1"/>
-      <c r="C102" s="1"/>
-      <c r="D102" s="1"/>
+      <c r="A102" s="1">
+        <v>799.59900000000005</v>
+      </c>
+      <c r="B102" s="1">
+        <v>842.99400000000003</v>
+      </c>
+      <c r="C102" s="1">
+        <v>2995.8</v>
+      </c>
+      <c r="D102" s="1">
+        <v>4.03</v>
+      </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A103" s="1"/>
-      <c r="B103" s="1"/>
-      <c r="C103" s="1"/>
-      <c r="D103" s="1"/>
+      <c r="A103" s="1">
+        <v>801.74</v>
+      </c>
+      <c r="B103" s="1">
+        <v>748.91700000000003</v>
+      </c>
+      <c r="C103" s="1">
+        <v>2995.8</v>
+      </c>
+      <c r="D103" s="1">
+        <v>6.03</v>
+      </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A104" s="1"/>
-      <c r="B104" s="1"/>
-      <c r="C104" s="1"/>
-      <c r="D104" s="1"/>
+      <c r="A104" s="1">
+        <v>804.21600000000001</v>
+      </c>
+      <c r="B104" s="1">
+        <v>653.74800000000005</v>
+      </c>
+      <c r="C104" s="1">
+        <v>2995.8</v>
+      </c>
+      <c r="D104" s="1">
+        <v>8.0299999999999994</v>
+      </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A105" s="1"/>
-      <c r="B105" s="1"/>
-      <c r="C105" s="1"/>
-      <c r="D105" s="1"/>
+      <c r="A105" s="1">
+        <v>807.50099999999998</v>
+      </c>
+      <c r="B105" s="1">
+        <v>559.178</v>
+      </c>
+      <c r="C105" s="1">
+        <v>2995.8</v>
+      </c>
+      <c r="D105" s="1">
+        <v>10.029999999999999</v>
+      </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A106" s="1"/>
-      <c r="B106" s="1"/>
-      <c r="C106" s="1"/>
-      <c r="D106" s="1"/>
+      <c r="A106" s="1">
+        <v>811.2</v>
+      </c>
+      <c r="B106" s="1">
+        <v>462.858</v>
+      </c>
+      <c r="C106" s="1">
+        <v>2995.8</v>
+      </c>
+      <c r="D106" s="1">
+        <v>12.03</v>
+      </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A107" s="1"/>
-      <c r="B107" s="1"/>
-      <c r="C107" s="1"/>
-      <c r="D107" s="1"/>
+      <c r="A107" s="1">
+        <v>815.16600000000005</v>
+      </c>
+      <c r="B107" s="1">
+        <v>365.44299999999998</v>
+      </c>
+      <c r="C107" s="1">
+        <v>2995.8</v>
+      </c>
+      <c r="D107" s="1">
+        <v>14.03</v>
+      </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A108" s="1"/>
-      <c r="B108" s="1"/>
-      <c r="C108" s="1"/>
-      <c r="D108" s="1"/>
+      <c r="A108" s="1">
+        <v>819.63599999999997</v>
+      </c>
+      <c r="B108" s="1">
+        <v>265.04700000000003</v>
+      </c>
+      <c r="C108" s="1">
+        <v>2995.8</v>
+      </c>
+      <c r="D108" s="1">
+        <v>16.03</v>
+      </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" s="1"/>

</xml_diff>